<commit_message>
some west end changes
</commit_message>
<xml_diff>
--- a/int_changes_barrens_forests.xlsx
+++ b/int_changes_barrens_forests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>Interaction Changes from Barrens to Forests</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Megastraea positively affected by juvenile mac in barrens, but negatively in forests</t>
   </si>
   <si>
-    <t>Megastraea negatively affected by laminaria and pterygophora. In forests the negative effect of laminaria is reduced, the negative effect of pterygophora is stronger</t>
-  </si>
-  <si>
     <t>Important observations</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t>Something with megastraea/juvenile mac/pter</t>
+  </si>
+  <si>
+    <t>Megastraea negatively affected by laminaria and pterygophora.</t>
+  </si>
+  <si>
+    <t>In forests the negative effect of laminaria is reduced, the negative effect of pterygophora is stronger</t>
   </si>
 </sst>
 </file>
@@ -182,14 +185,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -428,36 +431,91 @@
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -466,75 +524,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,777 +841,781 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="8" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="13.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="15" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:14" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="15" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="30"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="15" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="40"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="15" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="33"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="16"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="6"/>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="23"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="27"/>
-      <c r="J11" s="5" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+      <c r="J11" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="8"/>
-      <c r="J12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="17" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="15"/>
+      <c r="J12" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="17" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="J14" s="18" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J14" s="37" t="s">
         <v>21</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-    </row>
-    <row r="17" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="J16" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+    </row>
+    <row r="17" spans="1:14" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="36" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="29" t="s">
+      <c r="D17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="20" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-    </row>
-    <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="L17" s="40"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+    </row>
+    <row r="18" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="36" t="s">
+      <c r="B18" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="30" t="s">
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="J18" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="L18" s="20"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-    </row>
-    <row r="19" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+    </row>
+    <row r="19" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="34" t="s">
+      <c r="B19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="20" t="s">
+      <c r="H19" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-    </row>
-    <row r="20" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+    </row>
+    <row r="20" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="8" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="33" t="s">
+      <c r="G20" s="25"/>
+      <c r="H20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="J20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-    </row>
-    <row r="21" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+    </row>
+    <row r="21" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="s">
+      <c r="B21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="21" t="s">
+      <c r="E21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="20"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-    </row>
-    <row r="22" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+    </row>
+    <row r="22" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="35" t="s">
+      <c r="B22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="21" t="s">
+      <c r="H22" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="20"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-    </row>
-    <row r="23" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="34" t="s">
+      <c r="B23" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="21" t="s">
+      <c r="H23" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="L23" s="20"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-    </row>
-    <row r="24" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="L23" s="40"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="8"/>
-      <c r="K24" s="21" t="s">
+      <c r="H24" s="15"/>
+      <c r="J24" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="21" t="s">
+      <c r="J25" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="L25" s="20"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L25" s="40"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="J26" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="L26" s="20"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+    </row>
+    <row r="27" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K27" s="43" t="s">
+      <c r="J27" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L27" s="20"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-    </row>
-    <row r="28" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="L27" s="40"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+    </row>
+    <row r="28" spans="1:14" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="K28" s="21" t="s">
+      <c r="B28" s="8"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="J28" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="L28" s="20"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-    </row>
-    <row r="29" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="L28" s="40"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+    </row>
+    <row r="29" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="30"/>
-      <c r="K29" s="21" t="s">
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21"/>
+      <c r="J29" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="L29" s="20"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-    </row>
-    <row r="30" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+    </row>
+    <row r="30" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="41"/>
-      <c r="K30" s="21" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="33"/>
+      <c r="J30" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="L30" s="20"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-    </row>
-    <row r="31" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+    </row>
+    <row r="31" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="33"/>
-      <c r="K31" s="21" t="s">
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="16"/>
+      <c r="J31" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+    </row>
+    <row r="32" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="23"/>
+      <c r="J32" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="40"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+    </row>
+    <row r="33" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="34"/>
+      <c r="J33" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="L33" s="40"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="15"/>
+      <c r="J34" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="J35" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J36" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="40"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J37" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J38" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="L38" s="40"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J39" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-    </row>
-    <row r="32" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="6"/>
-      <c r="K32" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="L32" s="20"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-    </row>
-    <row r="33" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="27"/>
-      <c r="K33" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="L33" s="20"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-    </row>
-    <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="8"/>
-      <c r="K34" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="20"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-    </row>
-    <row r="35" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="K35" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="L35" s="20"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K37" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K38" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="L38" s="20"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K39" s="44" t="s">
+      <c r="L39" s="40"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J40" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="L39" s="20"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K40" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="L40" s="20"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K42" s="20"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="21"/>
-      <c r="N45" s="21"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K46" s="20"/>
-      <c r="L46" s="21"/>
-      <c r="M46" s="21"/>
-      <c r="N46" s="21"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="21"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K48" s="20"/>
-      <c r="L48" s="20"/>
-      <c r="M48" s="21"/>
-      <c r="N48" s="21"/>
-    </row>
-    <row r="49" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K49" s="20"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="21"/>
-    </row>
-    <row r="50" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="21"/>
-    </row>
-    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K51" s="20"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-    </row>
-    <row r="52" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K52" s="20"/>
-    </row>
-    <row r="53" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K53" s="20"/>
-    </row>
-    <row r="54" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K54" s="20"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K42" s="40"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K46" s="40"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="41"/>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K49" s="40"/>
+      <c r="L49" s="41"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="41"/>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="41"/>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K51" s="40"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K52" s="40"/>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K53" s="40"/>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K54" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>